<commit_message>
Creation menu app + image premier livre
</commit_message>
<xml_diff>
--- a/doc/journalTravail.xlsx
+++ b/doc/journalTravail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\passionLecture\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1A004D-9F98-4B6A-9981-B6D02FDBA739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9DBA0A-E39C-45EF-A1EA-9D9406A885C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="75" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Modifications de la maquette LivreChoisi + création de la maquette GestTag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apprentissage des base de MAUI création du menu de l'app plus photo du prmier livre </t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1039,7 @@
                   <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.10416666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1965,9 +1968,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2020,7 +2023,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 3 heurs 50 minutes</v>
+        <v>0 jours 6 heurs 20 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2035,15 +2038,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="25">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>230</v>
+        <v>380</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2202,10 +2205,21 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="43"/>
-      <c r="F12" s="48"/>
+      <c r="B12" s="39">
+        <v>45376</v>
+      </c>
+      <c r="C12" s="35">
+        <v>2</v>
+      </c>
+      <c r="D12" s="43">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>34</v>
+      </c>
       <c r="G12" s="17"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -8189,11 +8203,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8201,7 +8215,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8310,7 +8324,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>7.6388888888888881E-2</v>
+        <v>0.18055555555555555</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8332,18 +8346,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="19" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f3418dd4ca302601ba73fa17965a3f21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns4="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d82fd028d299635ce1df2d808d1b2ae" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8609,6 +8611,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -8618,20 +8632,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AC923F-FD8C-4D8C-BC85-CA1561E8B39C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8649,4 +8649,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implémentation liste  image dans livre
</commit_message>
<xml_diff>
--- a/doc/journalTravail.xlsx
+++ b/doc/journalTravail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\passionLecture\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9DBA0A-E39C-45EF-A1EA-9D9406A885C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6281919-D236-4A28-A894-CAF1AE9AD3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="75" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -144,7 +144,22 @@
     <t>Modifications de la maquette LivreChoisi + création de la maquette GestTag</t>
   </si>
   <si>
-    <t xml:space="preserve">Apprentissage des base de MAUI création du menu de l'app plus photo du prmier livre </t>
+    <t>Revue du code avant les vacances + aide mathis car absent avant vacance</t>
+  </si>
+  <si>
+    <t>Changement du TAbBar afin qu'il ne prennne pas de marge sur l'application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apprentissage des base de MAUI création du menu de l'app plus photo du premier livre </t>
+  </si>
+  <si>
+    <t>début d'ajout de l'affichage de la liste des livre dans la page livre</t>
+  </si>
+  <si>
+    <t>toilet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essaie d'implémentation d'une lise d'image boutton dans la page Livre </t>
   </si>
 </sst>
 </file>
@@ -1036,10 +1051,10 @@
                 <c:formatCode>hh\ "h"\ mm\ "min"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>3.4722222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10416666666666667</c:v>
+                  <c:v>0.22222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1057,7 +1072,7 @@
                   <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1968,9 +1983,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2023,7 +2038,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 6 heurs 20 minutes</v>
+        <v>0 jours 9 heurs 40 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2038,15 +2053,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="25">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>140</v>
+        <v>220</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>380</v>
+        <v>580</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2218,7 +2233,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="48" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G12" s="17"/>
       <c r="M12" t="s">
@@ -2233,11 +2248,19 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
-      <c r="B13" s="40"/>
+      <c r="B13" s="40">
+        <v>45397</v>
+      </c>
       <c r="C13" s="36"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="48"/>
+      <c r="D13" s="44">
+        <v>20</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>34</v>
+      </c>
       <c r="G13" s="20"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2252,8 +2275,15 @@
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="39"/>
       <c r="C14" s="35"/>
-      <c r="D14" s="43"/>
-      <c r="F14" s="48"/>
+      <c r="D14" s="43">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>35</v>
+      </c>
       <c r="G14" s="17"/>
       <c r="M14" t="s">
         <v>24</v>
@@ -2269,9 +2299,15 @@
       <c r="A15" s="18"/>
       <c r="B15" s="40"/>
       <c r="C15" s="36"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="48"/>
+      <c r="D15" s="44">
+        <v>10</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>37</v>
+      </c>
       <c r="G15" s="20"/>
       <c r="M15" t="s">
         <v>25</v>
@@ -2286,8 +2322,15 @@
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="39"/>
       <c r="C16" s="35"/>
-      <c r="D16" s="43"/>
-      <c r="F16" s="48"/>
+      <c r="D16" s="43">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="17"/>
       <c r="O16">
         <v>40</v>
@@ -2296,10 +2339,18 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="40"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="48"/>
+      <c r="C17" s="36">
+        <v>2</v>
+      </c>
+      <c r="D17" s="44">
+        <v>30</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>39</v>
+      </c>
       <c r="G17" s="20"/>
       <c r="O17">
         <v>45</v>
@@ -8189,7 +8240,7 @@
       </c>
       <c r="B4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C4" s="28" t="str">
         <f>'Journal de travail'!M8</f>
@@ -8197,17 +8248,17 @@
       </c>
       <c r="D4" s="45">
         <f>(A4+B4)/1440</f>
-        <v>2.0833333333333332E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8215,7 +8266,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.10416666666666667</v>
+        <v>0.22222222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8307,7 +8358,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="51" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8315,7 +8366,7 @@
       </c>
       <c r="D11" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8324,7 +8375,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.18055555555555555</v>
+        <v>0.31944444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8346,6 +8397,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="19" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f3418dd4ca302601ba73fa17965a3f21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns4="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d82fd028d299635ce1df2d808d1b2ae" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8611,18 +8674,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -8632,6 +8683,20 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AC923F-FD8C-4D8C-BC85-CA1561E8B39C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8649,18 +8714,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
restart ordi trop lent
</commit_message>
<xml_diff>
--- a/doc/journalTravail.xlsx
+++ b/doc/journalTravail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\passionLecture\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6D9DAD-3A47-409D-8F18-F031AB2A1F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879DAC6C-3B24-4A99-91B8-480F03E5EA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="75" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Tentative lire Epub depuis DB</t>
+  </si>
+  <si>
+    <t>récupération d'un epub depuis la base de donnée</t>
+  </si>
+  <si>
+    <t>Mise en place d'une route ne donnant que les titres dans l'API</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1099,7 @@
                   <c:v>3.4722222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57638888888888884</c:v>
+                  <c:v>0.61805555555555558</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2022,9 +2028,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2077,7 +2083,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 18 heurs 35 minutes</v>
+        <v>0 jours 19 heurs 34 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2096,11 +2102,11 @@
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>515</v>
+        <v>575</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>1115</v>
+        <v>1175</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2628,18 +2634,33 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
-      <c r="B33" s="40"/>
+      <c r="B33" s="40">
+        <v>45425</v>
+      </c>
       <c r="C33" s="36"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="47"/>
+      <c r="D33" s="44">
+        <v>25</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="47" t="s">
+        <v>53</v>
+      </c>
       <c r="G33" s="20"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="39"/>
       <c r="C34" s="35"/>
-      <c r="D34" s="43"/>
-      <c r="F34" s="47"/>
+      <c r="D34" s="43">
+        <v>35</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="47" t="s">
+        <v>54</v>
+      </c>
       <c r="G34" s="17"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -8403,7 +8424,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>350</v>
+        <v>410</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8411,7 +8432,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.57638888888888884</v>
+        <v>0.61805555555555558</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8520,7 +8541,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.69097222222222221</v>
+        <v>0.73263888888888895</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8542,6 +8563,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="19" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f3418dd4ca302601ba73fa17965a3f21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns4="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d82fd028d299635ce1df2d808d1b2ae" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8807,18 +8840,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -8828,6 +8849,20 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AC923F-FD8C-4D8C-BC85-CA1561E8B39C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8845,18 +8880,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>